<commit_message>
Fix bugs with Hex. Fixes for writing gamma.csv, hxs.csv, vol.csv. Passes tests for meoh+cyclo Hex, CaseStudy1. Improved prompting for input files to ensure that file exist. Fix typos in database files for meoh_cyclo and CaseStudy1.
Signed-off-by: Carl Lira <lira@msu.edu>
</commit_message>
<xml_diff>
--- a/Input/GAMMAPA/Database - Pure and Site param.xlsx
+++ b/Input/GAMMAPA/Database - Pure and Site param.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lira.EGR\Documents\repos\MDNAproject\Input\GAMMAPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154A2EB0-8DB6-4D51-AC55-1D6374A1F265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88503EEA-31FC-451A-8ED7-7D174945B5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="713" activeTab="11" xr2:uid="{F5CC7CA9-1E49-41AC-B255-1C67DD959E18}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="161">
   <si>
     <t>site id</t>
   </si>
@@ -515,6 +515,18 @@
   </si>
   <si>
     <t>This table is used to collect ID number as pasted from ../IdTrcDipCas.txt. The row order is not important, only the column order. Add components as needed.</t>
+  </si>
+  <si>
+    <t>vdw, not realistic, just for testing/benchmarking code, CaseStudy1</t>
+  </si>
+  <si>
+    <t>vdw, not realistic, just for testing/benchmarking code, CaseStudy2</t>
+  </si>
+  <si>
+    <t>vdw, not realistic, just for testing/benchmarking code, CaseStudy3</t>
+  </si>
+  <si>
+    <t>not realistic, used only for testing/benchmarking, CaseStudy1</t>
   </si>
 </sst>
 </file>
@@ -1431,8 +1443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8459BD88-E818-403A-9C78-0332BC51A281}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1450,14 +1462,17 @@
       <c r="F1" t="s">
         <v>71</v>
       </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
+        <v>123</v>
       </c>
       <c r="J1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="K1" t="s">
         <v>88</v>
@@ -1492,17 +1507,20 @@
         <f>_xlfn.XLOOKUP(vdW!D3,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
         <v>METHANOL</v>
       </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
       <c r="H3">
-        <v>20</v>
+        <v>100.2</v>
       </c>
       <c r="I3">
-        <v>100.2</v>
-      </c>
-      <c r="J3">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>160</v>
       </c>
       <c r="K3" t="str">
-        <f>_xlfn.XLOOKUP(J3,sources!A$2:A$40,sources!C$2:C$40)</f>
+        <f>_xlfn.XLOOKUP(I3,sources!A$2:A$40,sources!C$2:C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
@@ -1524,17 +1542,20 @@
         <f>_xlfn.XLOOKUP(vdW!D4,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
         <v>ETHANOL</v>
       </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
       <c r="H4">
-        <v>30</v>
+        <v>100.2</v>
       </c>
       <c r="I4">
-        <v>100.2</v>
-      </c>
-      <c r="J4">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
+        <v>160</v>
       </c>
       <c r="K4" t="str">
-        <f>_xlfn.XLOOKUP(J4,sources!A$2:A$40,sources!C$2:C$40)</f>
+        <f>_xlfn.XLOOKUP(I4,sources!A$2:A$40,sources!C$2:C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
@@ -1702,23 +1723,26 @@
         <v>METHANOL</v>
       </c>
       <c r="D13">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="E13" t="str">
         <f>_xlfn.XLOOKUP(vdW!D13,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>ETHANOL</v>
+      </c>
+      <c r="G13">
+        <v>25</v>
       </c>
       <c r="H13">
-        <v>25</v>
+        <v>100.2</v>
       </c>
       <c r="I13">
-        <v>100.2</v>
-      </c>
-      <c r="J13">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="J13" t="s">
+        <v>160</v>
       </c>
       <c r="K13" t="str">
-        <f>_xlfn.XLOOKUP(J13,sources!A$2:A$40,sources!C$2:C$40)</f>
+        <f>_xlfn.XLOOKUP(I13,sources!A$2:A$40,sources!C$2:C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
@@ -1740,17 +1764,20 @@
         <f>_xlfn.XLOOKUP(vdW!D14,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
         <v>METHANOL</v>
       </c>
+      <c r="G14">
+        <v>35</v>
+      </c>
       <c r="H14">
-        <v>35</v>
+        <v>100.2</v>
       </c>
       <c r="I14">
-        <v>100.2</v>
-      </c>
-      <c r="J14">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="J14" t="s">
+        <v>160</v>
       </c>
       <c r="K14" t="str">
-        <f>_xlfn.XLOOKUP(J14,sources!A$2:A$40,sources!C$2:C$40)</f>
+        <f>_xlfn.XLOOKUP(I14,sources!A$2:A$40,sources!C$2:C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
@@ -1761,15 +1788,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2374B1E-7050-450D-B3AF-CF5254FCED57}">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1792,10 +1819,13 @@
         <v>122</v>
       </c>
       <c r="M1" t="s">
+        <v>126</v>
+      </c>
+      <c r="N1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1806,7 +1836,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1833,12 +1863,12 @@
       <c r="L3">
         <v>16</v>
       </c>
-      <c r="M3" t="str">
+      <c r="N3" t="str">
         <f>_xlfn.XLOOKUP(L3,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark1 - distributed with 2.6.5rel</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1857,7 +1887,7 @@
         <v>ETHANOL</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1876,7 +1906,7 @@
         <v>1-PROPANOL</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1895,7 +1925,7 @@
         <v>1-BUTANOL</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1914,7 +1944,7 @@
         <v>1-PENTANOL</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1933,7 +1963,7 @@
         <v>1-HEXANOL</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1952,7 +1982,7 @@
         <v>2-METHYL-1-PROPANOL</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1971,7 +2001,7 @@
         <v>ISOPROPANOL</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1990,7 +2020,7 @@
         <v>2-BUTANOL</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2009,7 +2039,7 @@
         <v>2-METHYL-2-PROPANOL</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2028,7 +2058,7 @@
         <v>METHANOL</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2047,7 +2077,7 @@
         <v>METHANOL</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2074,12 +2104,12 @@
       <c r="L15">
         <v>17</v>
       </c>
-      <c r="M15" t="str">
+      <c r="N15" t="str">
         <f>_xlfn.XLOOKUP(L15,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2106,12 +2136,12 @@
       <c r="L16">
         <v>17</v>
       </c>
-      <c r="M16" t="str">
+      <c r="N16" t="str">
         <f>_xlfn.XLOOKUP(L16,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2138,12 +2168,12 @@
       <c r="L17">
         <v>17</v>
       </c>
-      <c r="M17" t="str">
+      <c r="N17" t="str">
         <f>_xlfn.XLOOKUP(L17,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2170,12 +2200,12 @@
       <c r="L18">
         <v>17</v>
       </c>
-      <c r="M18" t="str">
+      <c r="N18" t="str">
         <f>_xlfn.XLOOKUP(L18,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2202,12 +2232,12 @@
       <c r="L19">
         <v>17</v>
       </c>
-      <c r="M19" t="str">
+      <c r="N19" t="str">
         <f>_xlfn.XLOOKUP(L19,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>17</v>
       </c>
@@ -2234,12 +2264,12 @@
       <c r="L20">
         <v>17</v>
       </c>
-      <c r="M20" t="str">
+      <c r="N20" t="str">
         <f>_xlfn.XLOOKUP(L20,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2266,12 +2296,12 @@
       <c r="L21">
         <v>17</v>
       </c>
-      <c r="M21" t="str">
+      <c r="N21" t="str">
         <f>_xlfn.XLOOKUP(L21,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>19</v>
       </c>
@@ -2298,12 +2328,12 @@
       <c r="L22">
         <v>17</v>
       </c>
-      <c r="M22" t="str">
+      <c r="N22" t="str">
         <f>_xlfn.XLOOKUP(L22,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>20</v>
       </c>
@@ -2330,12 +2360,12 @@
       <c r="L23">
         <v>17</v>
       </c>
-      <c r="M23" t="str">
+      <c r="N23" t="str">
         <f>_xlfn.XLOOKUP(L23,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>21</v>
       </c>
@@ -2362,12 +2392,12 @@
       <c r="L24">
         <v>17</v>
       </c>
-      <c r="M24" t="str">
+      <c r="N24" t="str">
         <f>_xlfn.XLOOKUP(L24,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>22</v>
       </c>
@@ -2394,12 +2424,12 @@
       <c r="L25">
         <v>17</v>
       </c>
-      <c r="M25" t="str">
+      <c r="N25" t="str">
         <f>_xlfn.XLOOKUP(L25,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>23</v>
       </c>
@@ -2426,12 +2456,12 @@
       <c r="L26">
         <v>17</v>
       </c>
-      <c r="M26" t="str">
+      <c r="N26" t="str">
         <f>_xlfn.XLOOKUP(L26,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>24</v>
       </c>
@@ -2458,12 +2488,12 @@
       <c r="L27">
         <v>17</v>
       </c>
-      <c r="M27" t="str">
+      <c r="N27" t="str">
         <f>_xlfn.XLOOKUP(L27,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>25</v>
       </c>
@@ -2490,12 +2520,12 @@
       <c r="L28">
         <v>17</v>
       </c>
-      <c r="M28" t="str">
+      <c r="N28" t="str">
         <f>_xlfn.XLOOKUP(L28,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>26</v>
       </c>
@@ -2522,12 +2552,12 @@
       <c r="L29">
         <v>17</v>
       </c>
-      <c r="M29" t="str">
+      <c r="N29" t="str">
         <f>_xlfn.XLOOKUP(L29,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2554,12 +2584,12 @@
       <c r="L30">
         <v>17</v>
       </c>
-      <c r="M30" t="str">
+      <c r="N30" t="str">
         <f>_xlfn.XLOOKUP(L30,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2586,12 +2616,12 @@
       <c r="L31">
         <v>17</v>
       </c>
-      <c r="M31" t="str">
+      <c r="N31" t="str">
         <f>_xlfn.XLOOKUP(L31,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2618,12 +2648,12 @@
       <c r="L32">
         <v>17</v>
       </c>
-      <c r="M32" t="str">
+      <c r="N32" t="str">
         <f>_xlfn.XLOOKUP(L32,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2650,12 +2680,12 @@
       <c r="L33">
         <v>17</v>
       </c>
-      <c r="M33" t="str">
+      <c r="N33" t="str">
         <f>_xlfn.XLOOKUP(L33,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>31</v>
       </c>
@@ -2682,12 +2712,12 @@
       <c r="L34">
         <v>17</v>
       </c>
-      <c r="M34" t="str">
+      <c r="N34" t="str">
         <f>_xlfn.XLOOKUP(L34,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>32</v>
       </c>
@@ -2714,12 +2744,12 @@
       <c r="L35">
         <v>17</v>
       </c>
-      <c r="M35" t="str">
+      <c r="N35" t="str">
         <f>_xlfn.XLOOKUP(L35,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>33</v>
       </c>
@@ -2746,12 +2776,12 @@
       <c r="L36">
         <v>17</v>
       </c>
-      <c r="M36" t="str">
+      <c r="N36" t="str">
         <f>_xlfn.XLOOKUP(L36,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>34</v>
       </c>
@@ -2778,12 +2808,12 @@
       <c r="L37">
         <v>17</v>
       </c>
-      <c r="M37" t="str">
+      <c r="N37" t="str">
         <f>_xlfn.XLOOKUP(L37,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>35</v>
       </c>
@@ -2810,12 +2840,12 @@
       <c r="L38">
         <v>17</v>
       </c>
-      <c r="M38" t="str">
+      <c r="N38" t="str">
         <f>_xlfn.XLOOKUP(L38,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>36</v>
       </c>
@@ -2842,7 +2872,7 @@
       <c r="L39">
         <v>17</v>
       </c>
-      <c r="M39" t="str">
+      <c r="N39" t="str">
         <f>_xlfn.XLOOKUP(L39,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
@@ -2857,7 +2887,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3015,7 +3045,7 @@
         <v>115</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="I5">
         <v>-100</v>
@@ -3024,7 +3054,7 @@
         <v>0.3</v>
       </c>
       <c r="K5" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="L5">
         <v>17</v>
@@ -3068,7 +3098,7 @@
         <v>0.3</v>
       </c>
       <c r="K6" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="L6">
         <v>17</v>
@@ -3112,7 +3142,7 @@
         <v>0.3</v>
       </c>
       <c r="K7" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="L7">
         <v>17</v>
@@ -3123,6 +3153,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3344,8 +3375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB1F51B-B386-419D-A013-864D12BA04CF}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4156,7 +4187,7 @@
   <dimension ref="A2:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C4" sqref="C4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4512,7 +4543,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E4"/>
+      <selection activeCell="A4" sqref="A4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4809,7 +4840,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E4"/>
+      <selection activeCell="A4" sqref="A4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5558,15 +5589,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CBBE5A-E8DE-4E54-B78F-49BA95C635AD}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -5592,10 +5623,13 @@
         <v>123</v>
       </c>
       <c r="M1" t="s">
+        <v>126</v>
+      </c>
+      <c r="N1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5606,7 +5640,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5633,12 +5667,12 @@
       <c r="L3">
         <v>16</v>
       </c>
-      <c r="M3" t="str">
+      <c r="N3" t="str">
         <f>_xlfn.XLOOKUP(L3,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark1 - distributed with 2.6.5rel</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5657,7 +5691,7 @@
         <v>ETHANOL</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5676,7 +5710,7 @@
         <v>1-PROPANOL</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5695,7 +5729,7 @@
         <v>1-BUTANOL</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5714,7 +5748,7 @@
         <v>1-PENTANOL</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5733,7 +5767,7 @@
         <v>1-HEXANOL</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5752,7 +5786,7 @@
         <v>2-METHYL-1-PROPANOL</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5771,7 +5805,7 @@
         <v>ISOPROPANOL</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5790,7 +5824,7 @@
         <v>2-BUTANOL</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5809,7 +5843,7 @@
         <v>2-METHYL-2-PROPANOL</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5836,12 +5870,12 @@
       <c r="L13">
         <v>17</v>
       </c>
-      <c r="M13" t="str">
+      <c r="N13" t="str">
         <f>_xlfn.XLOOKUP(L13,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5868,12 +5902,12 @@
       <c r="L14">
         <v>17</v>
       </c>
-      <c r="M14" t="str">
+      <c r="N14" t="str">
         <f>_xlfn.XLOOKUP(L14,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5900,12 +5934,12 @@
       <c r="L15">
         <v>17</v>
       </c>
-      <c r="M15" t="str">
+      <c r="N15" t="str">
         <f>_xlfn.XLOOKUP(L15,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5932,12 +5966,12 @@
       <c r="L16">
         <v>17</v>
       </c>
-      <c r="M16" t="str">
+      <c r="N16" t="str">
         <f>_xlfn.XLOOKUP(L16,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5964,12 +5998,12 @@
       <c r="L17">
         <v>17</v>
       </c>
-      <c r="M17" t="str">
+      <c r="N17" t="str">
         <f>_xlfn.XLOOKUP(L17,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5996,12 +6030,12 @@
       <c r="L18">
         <v>17</v>
       </c>
-      <c r="M18" t="str">
+      <c r="N18" t="str">
         <f>_xlfn.XLOOKUP(L18,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -6028,12 +6062,12 @@
       <c r="L19">
         <v>17</v>
       </c>
-      <c r="M19" t="str">
+      <c r="N19" t="str">
         <f>_xlfn.XLOOKUP(L19,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -6060,12 +6094,12 @@
       <c r="L20">
         <v>17</v>
       </c>
-      <c r="M20" t="str">
+      <c r="N20" t="str">
         <f>_xlfn.XLOOKUP(L20,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -6092,12 +6126,12 @@
       <c r="L21">
         <v>17</v>
       </c>
-      <c r="M21" t="str">
+      <c r="N21" t="str">
         <f>_xlfn.XLOOKUP(L21,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -6124,12 +6158,12 @@
       <c r="L22">
         <v>17</v>
       </c>
-      <c r="M22" t="str">
+      <c r="N22" t="str">
         <f>_xlfn.XLOOKUP(L22,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -6156,12 +6190,12 @@
       <c r="L23">
         <v>17</v>
       </c>
-      <c r="M23" t="str">
+      <c r="N23" t="str">
         <f>_xlfn.XLOOKUP(L23,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -6188,12 +6222,12 @@
       <c r="L24">
         <v>17</v>
       </c>
-      <c r="M24" t="str">
+      <c r="N24" t="str">
         <f>_xlfn.XLOOKUP(L24,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6220,12 +6254,12 @@
       <c r="L25">
         <v>17</v>
       </c>
-      <c r="M25" t="str">
+      <c r="N25" t="str">
         <f>_xlfn.XLOOKUP(L25,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6252,12 +6286,12 @@
       <c r="L26">
         <v>17</v>
       </c>
-      <c r="M26" t="str">
+      <c r="N26" t="str">
         <f>_xlfn.XLOOKUP(L26,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -6284,12 +6318,12 @@
       <c r="L27">
         <v>17</v>
       </c>
-      <c r="M27" t="str">
+      <c r="N27" t="str">
         <f>_xlfn.XLOOKUP(L27,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -6316,12 +6350,12 @@
       <c r="L28">
         <v>17</v>
       </c>
-      <c r="M28" t="str">
+      <c r="N28" t="str">
         <f>_xlfn.XLOOKUP(L28,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -6348,12 +6382,12 @@
       <c r="L29">
         <v>17</v>
       </c>
-      <c r="M29" t="str">
+      <c r="N29" t="str">
         <f>_xlfn.XLOOKUP(L29,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -6380,12 +6414,12 @@
       <c r="L30">
         <v>17</v>
       </c>
-      <c r="M30" t="str">
+      <c r="N30" t="str">
         <f>_xlfn.XLOOKUP(L30,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -6412,12 +6446,12 @@
       <c r="L31">
         <v>17</v>
       </c>
-      <c r="M31" t="str">
+      <c r="N31" t="str">
         <f>_xlfn.XLOOKUP(L31,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -6444,12 +6478,12 @@
       <c r="L32">
         <v>17</v>
       </c>
-      <c r="M32" t="str">
+      <c r="N32" t="str">
         <f>_xlfn.XLOOKUP(L32,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -6476,12 +6510,12 @@
       <c r="L33">
         <v>17</v>
       </c>
-      <c r="M33" t="str">
+      <c r="N33" t="str">
         <f>_xlfn.XLOOKUP(L33,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -6508,12 +6542,12 @@
       <c r="L34">
         <v>17</v>
       </c>
-      <c r="M34" t="str">
+      <c r="N34" t="str">
         <f>_xlfn.XLOOKUP(L34,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -6540,12 +6574,12 @@
       <c r="L35">
         <v>17</v>
       </c>
-      <c r="M35" t="str">
+      <c r="N35" t="str">
         <f>_xlfn.XLOOKUP(L35,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -6572,12 +6606,12 @@
       <c r="L36">
         <v>17</v>
       </c>
-      <c r="M36" t="str">
+      <c r="N36" t="str">
         <f>_xlfn.XLOOKUP(L36,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -6604,7 +6638,7 @@
       <c r="L37">
         <v>17</v>
       </c>
-      <c r="M37" t="str">
+      <c r="N37" t="str">
         <f>_xlfn.XLOOKUP(L37,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>

</xml_diff>

<commit_message>
No calculational code changes. Cosmetic changes. Update parameter database. Additional benchmark files. Code passes benchmarks 2i, 2v, 2ix.
Signed-off-by: Lira, Carl <lira@msu.edu>
</commit_message>
<xml_diff>
--- a/Input/GAMMAPA/Database - Pure and Site param.xlsx
+++ b/Input/GAMMAPA/Database - Pure and Site param.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lira.EGR\Documents\repos\MDNAproject\Input\GAMMAPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88503EEA-31FC-451A-8ED7-7D174945B5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6255C3A-90C9-43ED-8CCA-29759BD4DC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="713" activeTab="11" xr2:uid="{F5CC7CA9-1E49-41AC-B255-1C67DD959E18}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="713" activeTab="11" xr2:uid="{F5CC7CA9-1E49-41AC-B255-1C67DD959E18}"/>
   </bookViews>
   <sheets>
     <sheet name="ID ref" sheetId="10" r:id="rId1"/>
@@ -981,7 +981,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1790,7 +1790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2374B1E-7050-450D-B3AF-CF5254FCED57}">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -3376,7 +3376,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:F15"/>
+      <selection activeCell="B16" sqref="B16:M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4187,7 +4187,7 @@
   <dimension ref="A2:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:J4"/>
+      <selection activeCell="C6" sqref="C6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4543,7 +4543,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E5"/>
+      <selection activeCell="A16" sqref="A16:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4607,7 +4607,7 @@
         <v>5350</v>
       </c>
       <c r="D4" t="str">
-        <f>_xlfn.XLOOKUP(ea!C4,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C4,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>METHANOL</v>
       </c>
       <c r="E4">
@@ -4625,7 +4625,7 @@
         <v>5245</v>
       </c>
       <c r="D5" t="str">
-        <f>_xlfn.XLOOKUP(ed!C5,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C5,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>ETHANOL</v>
       </c>
       <c r="E5">
@@ -4643,7 +4643,7 @@
         <v>5514</v>
       </c>
       <c r="D6" t="str">
-        <f>_xlfn.XLOOKUP(ed!C6,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C6,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>1-PROPANOL</v>
       </c>
       <c r="E6">
@@ -4661,7 +4661,7 @@
         <v>5520</v>
       </c>
       <c r="D7" t="str">
-        <f>_xlfn.XLOOKUP(ed!C7,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C7,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>1-BUTANOL</v>
       </c>
       <c r="E7">
@@ -4679,7 +4679,7 @@
         <v>5521</v>
       </c>
       <c r="D8" t="str">
-        <f>_xlfn.XLOOKUP(ed!C8,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C8,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>1-PENTANOL</v>
       </c>
       <c r="E8">
@@ -4697,7 +4697,7 @@
         <v>742</v>
       </c>
       <c r="D9" t="str">
-        <f>_xlfn.XLOOKUP(ed!C9,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C9,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>1-HEXANOL</v>
       </c>
       <c r="E9">
@@ -4715,7 +4715,7 @@
         <v>5892</v>
       </c>
       <c r="D10" t="str">
-        <f>_xlfn.XLOOKUP(ed!C10,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C10,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>2-METHYL-1-PROPANOL</v>
       </c>
       <c r="E10">
@@ -4733,7 +4733,7 @@
         <v>5352</v>
       </c>
       <c r="D11" t="str">
-        <f>_xlfn.XLOOKUP(ed!C11,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C11,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>ISOPROPANOL</v>
       </c>
       <c r="E11">
@@ -4751,7 +4751,7 @@
         <v>5898</v>
       </c>
       <c r="D12" t="str">
-        <f>_xlfn.XLOOKUP(ed!C12,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C12,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>2-BUTANOL</v>
       </c>
       <c r="E12">
@@ -4769,7 +4769,7 @@
         <v>5673</v>
       </c>
       <c r="D13" t="str">
-        <f>_xlfn.XLOOKUP(ed!C13,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C13,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>2-METHYL-2-PROPANOL</v>
       </c>
       <c r="E13">
@@ -4787,7 +4787,7 @@
         <v>1122</v>
       </c>
       <c r="D14" t="str">
-        <f>_xlfn.XLOOKUP(ed!C14,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C14,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>1,4-DIOXANE</v>
       </c>
       <c r="E14">
@@ -4805,7 +4805,7 @@
         <v>7609</v>
       </c>
       <c r="D15" t="str">
-        <f>_xlfn.XLOOKUP(ed!C15,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C15,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="E15">
@@ -4823,7 +4823,7 @@
         <v>5822</v>
       </c>
       <c r="D16" t="str">
-        <f>_xlfn.XLOOKUP(ed!C16,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C16,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>WATER</v>
       </c>
       <c r="E16">
@@ -4840,7 +4840,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E5"/>
+      <selection activeCell="A16" sqref="A16:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4904,7 +4904,7 @@
         <v>5350</v>
       </c>
       <c r="D4" t="str">
-        <f>_xlfn.XLOOKUP(ea!C4,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C4,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>METHANOL</v>
       </c>
       <c r="E4">
@@ -4922,7 +4922,7 @@
         <v>5245</v>
       </c>
       <c r="D5" t="str">
-        <f>_xlfn.XLOOKUP(ea!C5,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C5,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>ETHANOL</v>
       </c>
       <c r="E5">
@@ -4940,7 +4940,7 @@
         <v>5514</v>
       </c>
       <c r="D6" t="str">
-        <f>_xlfn.XLOOKUP(ea!C6,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C6,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>1-PROPANOL</v>
       </c>
       <c r="E6">
@@ -4958,7 +4958,7 @@
         <v>5520</v>
       </c>
       <c r="D7" t="str">
-        <f>_xlfn.XLOOKUP(ea!C7,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C7,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>1-BUTANOL</v>
       </c>
       <c r="E7">
@@ -4976,7 +4976,7 @@
         <v>5521</v>
       </c>
       <c r="D8" t="str">
-        <f>_xlfn.XLOOKUP(ea!C8,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C8,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>1-PENTANOL</v>
       </c>
       <c r="E8">
@@ -4994,7 +4994,7 @@
         <v>742</v>
       </c>
       <c r="D9" t="str">
-        <f>_xlfn.XLOOKUP(ea!C9,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C9,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>1-HEXANOL</v>
       </c>
       <c r="E9">
@@ -5012,7 +5012,7 @@
         <v>5892</v>
       </c>
       <c r="D10" t="str">
-        <f>_xlfn.XLOOKUP(ea!C10,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C10,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>2-METHYL-1-PROPANOL</v>
       </c>
       <c r="E10">
@@ -5030,7 +5030,7 @@
         <v>5352</v>
       </c>
       <c r="D11" t="str">
-        <f>_xlfn.XLOOKUP(ea!C11,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C11,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>ISOPROPANOL</v>
       </c>
       <c r="E11">
@@ -5048,7 +5048,7 @@
         <v>5898</v>
       </c>
       <c r="D12" t="str">
-        <f>_xlfn.XLOOKUP(ea!C12,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C12,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>2-BUTANOL</v>
       </c>
       <c r="E12">
@@ -5066,7 +5066,7 @@
         <v>5673</v>
       </c>
       <c r="D13" t="str">
-        <f>_xlfn.XLOOKUP(ea!C13,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C13,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>2-METHYL-2-PROPANOL</v>
       </c>
       <c r="E13">
@@ -5084,11 +5084,11 @@
         <v>5355</v>
       </c>
       <c r="D14" t="str">
-        <f>_xlfn.XLOOKUP(ea!C14,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C14,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>CHLOROFORM</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -5102,7 +5102,7 @@
         <v>7609</v>
       </c>
       <c r="D15" t="str">
-        <f>_xlfn.XLOOKUP(ea!C15,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C15,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="E15">
@@ -5120,7 +5120,7 @@
         <v>5822</v>
       </c>
       <c r="D16" t="str">
-        <f>_xlfn.XLOOKUP(ea!C16,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C16,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>WATER</v>
       </c>
       <c r="E16">
@@ -5137,7 +5137,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5198,7 +5198,7 @@
         <v>5247</v>
       </c>
       <c r="D4" t="str">
-        <f>_xlfn.XLOOKUP(eda!C4,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
+        <f>_xlfn.XLOOKUP(C4,'ID ref'!$A$3:$A$500,'ID ref'!$D$3:$D$500)</f>
         <v>ACETIC ACID</v>
       </c>
       <c r="E4">
@@ -5591,8 +5591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CBBE5A-E8DE-4E54-B78F-49BA95C635AD}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Combine code into a single file. Execution verified for NRTL. Added loadWilson, loadSH, loadNagata, but those are untested.
Move source file to SourceCode2a and VS project files
to the project root.

Signed-off-by: Lira, Carl <lira@msu.edu>
</commit_message>
<xml_diff>
--- a/Input/GAMMAPA/Database - Pure and Site param.xlsx
+++ b/Input/GAMMAPA/Database - Pure and Site param.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lira.EGR\Documents\repos\MDNAproject\Input\GAMMAPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6255C3A-90C9-43ED-8CCA-29759BD4DC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B637A5-7B48-477F-9C28-D053EF1051A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="713" activeTab="11" xr2:uid="{F5CC7CA9-1E49-41AC-B255-1C67DD959E18}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="713" activeTab="11" xr2:uid="{F5CC7CA9-1E49-41AC-B255-1C67DD959E18}"/>
   </bookViews>
   <sheets>
     <sheet name="ID ref" sheetId="10" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="185">
   <si>
     <t>site id</t>
   </si>
@@ -52,12 +52,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>hydroxyl O</t>
-  </si>
-  <si>
-    <t>hydroxyl H</t>
-  </si>
-  <si>
     <t>electron donor sites</t>
   </si>
   <si>
@@ -439,24 +433,12 @@
     <t>hostname</t>
   </si>
   <si>
-    <t>ether O</t>
-  </si>
-  <si>
-    <t>water O</t>
-  </si>
-  <si>
     <t>noccur</t>
   </si>
   <si>
     <t>comments</t>
   </si>
   <si>
-    <t>chloroform H</t>
-  </si>
-  <si>
-    <t>water H</t>
-  </si>
-  <si>
     <t>r UNIQUAC</t>
   </si>
   <si>
@@ -527,6 +509,96 @@
   </si>
   <si>
     <t>not realistic, used only for testing/benchmarking, CaseStudy1</t>
+  </si>
+  <si>
+    <t>hydroxyl_H_MeOH</t>
+  </si>
+  <si>
+    <t>hydroxyl_H_generic</t>
+  </si>
+  <si>
+    <t>hydroxyl_H_EtOH</t>
+  </si>
+  <si>
+    <t>hydroxyl_H_C3OH</t>
+  </si>
+  <si>
+    <t>hydroxyl_H_C4OH</t>
+  </si>
+  <si>
+    <t>hydroxyl_H_C5OH</t>
+  </si>
+  <si>
+    <t>hydroxyl_H_C6OH</t>
+  </si>
+  <si>
+    <t>hydroxyl_H_ibutOH</t>
+  </si>
+  <si>
+    <t>hydroxyl_H_ipa</t>
+  </si>
+  <si>
+    <t>hydroxyl_H_tbut</t>
+  </si>
+  <si>
+    <t>chloroform_H</t>
+  </si>
+  <si>
+    <t>hydroxyl_H_EG</t>
+  </si>
+  <si>
+    <t>water_H_water</t>
+  </si>
+  <si>
+    <t>hydroxyl_O_MeOH</t>
+  </si>
+  <si>
+    <t>hydroxyl_O_EtOH</t>
+  </si>
+  <si>
+    <t>hydroxyl_O_C3OH</t>
+  </si>
+  <si>
+    <t>hydroxyl_O_C4OH</t>
+  </si>
+  <si>
+    <t>hydroxyl_O_C5OH</t>
+  </si>
+  <si>
+    <t>hydroxyl_O_C6OH</t>
+  </si>
+  <si>
+    <t>hydroxyl_O_ibutOH</t>
+  </si>
+  <si>
+    <t>hydroxyl_O_ipa</t>
+  </si>
+  <si>
+    <t>hydroxyl_O_tbut</t>
+  </si>
+  <si>
+    <t>hydroxyl_O_EG</t>
+  </si>
+  <si>
+    <t>1,4dioxane_O</t>
+  </si>
+  <si>
+    <t>water_O</t>
+  </si>
+  <si>
+    <t>hydroxyl_O_generic</t>
+  </si>
+  <si>
+    <t>hydroxyl_O_2-buOH</t>
+  </si>
+  <si>
+    <t>acetic acid</t>
+  </si>
+  <si>
+    <t>hydroxyl_H_2-buOH</t>
+  </si>
+  <si>
+    <t>These are shown to distinguish the association type. When inserting in the input file, collapse blank cells.</t>
   </si>
 </sst>
 </file>
@@ -991,27 +1063,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F2" t="s">
         <v>60</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1025,13 +1097,13 @@
         <v>67561</v>
       </c>
       <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
         <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1045,13 +1117,13 @@
         <v>64175</v>
       </c>
       <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
         <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1065,13 +1137,13 @@
         <v>71238</v>
       </c>
       <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
         <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1085,13 +1157,13 @@
         <v>67630</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1105,13 +1177,13 @@
         <v>71363</v>
       </c>
       <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
         <v>37</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1125,13 +1197,13 @@
         <v>78831</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -1145,13 +1217,13 @@
         <v>78922</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1165,13 +1237,13 @@
         <v>75650</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -1185,13 +1257,13 @@
         <v>71410</v>
       </c>
       <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
         <v>46</v>
-      </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1205,13 +1277,13 @@
         <v>6032297</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1225,13 +1297,13 @@
         <v>75854</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -1245,13 +1317,13 @@
         <v>137326</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1265,13 +1337,13 @@
         <v>75843</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1285,13 +1357,13 @@
         <v>111273</v>
       </c>
       <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" t="s">
         <v>57</v>
-      </c>
-      <c r="E16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1305,13 +1377,13 @@
         <v>110827</v>
       </c>
       <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" t="s">
         <v>63</v>
-      </c>
-      <c r="E17" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1325,13 +1397,13 @@
         <v>142825</v>
       </c>
       <c r="D18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" t="s">
         <v>66</v>
-      </c>
-      <c r="E18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1345,13 +1417,13 @@
         <v>64197</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -1365,13 +1437,13 @@
         <v>123911</v>
       </c>
       <c r="D20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" t="s">
         <v>75</v>
-      </c>
-      <c r="E20" t="s">
-        <v>76</v>
-      </c>
-      <c r="F20" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -1385,13 +1457,13 @@
         <v>67663</v>
       </c>
       <c r="D21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" t="s">
         <v>78</v>
-      </c>
-      <c r="E21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F21" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -1405,13 +1477,13 @@
         <v>107211</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -1425,13 +1497,13 @@
         <v>7732185</v>
       </c>
       <c r="D23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" t="s">
         <v>84</v>
-      </c>
-      <c r="E23" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1441,109 +1513,77 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8459BD88-E818-403A-9C78-0332BC51A281}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" t="s">
         <v>69</v>
       </c>
-      <c r="D1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" t="s">
-        <v>126</v>
-      </c>
-      <c r="K1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>501</v>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="str">
-        <f>_xlfn.XLOOKUP(vdW!B3,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>502</v>
-      </c>
-      <c r="E3" t="str">
-        <f>_xlfn.XLOOKUP(vdW!D3,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>METHANOL</v>
-      </c>
-      <c r="G3">
-        <v>20</v>
-      </c>
-      <c r="H3">
-        <v>100.2</v>
-      </c>
-      <c r="I3">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>160</v>
-      </c>
-      <c r="K3" t="str">
-        <f>_xlfn.XLOOKUP(I3,sources!A$2:A$40,sources!C$2:C$40)</f>
-        <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="str">
         <f>_xlfn.XLOOKUP(vdW!B4,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>ETHANOL</v>
+        <v>METHANOL</v>
       </c>
       <c r="D4">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E4" t="str">
         <f>_xlfn.XLOOKUP(vdW!D4,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ETHANOL</v>
+        <v>METHANOL</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H4">
         <v>100.2</v>
@@ -1552,7 +1592,7 @@
         <v>17</v>
       </c>
       <c r="J4" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="K4" t="str">
         <f>_xlfn.XLOOKUP(I4,sources!A$2:A$40,sources!C$2:C$40)</f>
@@ -1561,211 +1601,211 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="str">
         <f>_xlfn.XLOOKUP(vdW!B5,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1-PROPANOL</v>
+        <v>ETHANOL</v>
       </c>
       <c r="D5">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E5" t="str">
         <f>_xlfn.XLOOKUP(vdW!D5,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>1-PROPANOL</v>
+        <v>ETHANOL</v>
+      </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
+      <c r="H5">
+        <v>100.2</v>
+      </c>
+      <c r="I5">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>154</v>
+      </c>
+      <c r="K5" t="str">
+        <f>_xlfn.XLOOKUP(I5,sources!A$2:A$40,sources!C$2:C$40)</f>
+        <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="str">
         <f>_xlfn.XLOOKUP(vdW!B6,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1-BUTANOL</v>
+        <v>1-PROPANOL</v>
       </c>
       <c r="D6">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E6" t="str">
         <f>_xlfn.XLOOKUP(vdW!D6,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>1-BUTANOL</v>
+        <v>1-PROPANOL</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="str">
         <f>_xlfn.XLOOKUP(vdW!B7,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1-PENTANOL</v>
+        <v>1-BUTANOL</v>
       </c>
       <c r="D7">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E7" t="str">
         <f>_xlfn.XLOOKUP(vdW!D7,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>1-PENTANOL</v>
+        <v>1-BUTANOL</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.XLOOKUP(vdW!B8,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1-HEXANOL</v>
+        <v>1-PENTANOL</v>
       </c>
       <c r="D8">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E8" t="str">
         <f>_xlfn.XLOOKUP(vdW!D8,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>1-HEXANOL</v>
+        <v>1-PENTANOL</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="str">
         <f>_xlfn.XLOOKUP(vdW!B9,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>2-METHYL-1-PROPANOL</v>
+        <v>1-HEXANOL</v>
       </c>
       <c r="D9">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E9" t="str">
         <f>_xlfn.XLOOKUP(vdW!D9,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>2-METHYL-1-PROPANOL</v>
+        <v>1-HEXANOL</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="str">
         <f>_xlfn.XLOOKUP(vdW!B10,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>ISOPROPANOL</v>
+        <v>2-METHYL-1-PROPANOL</v>
       </c>
       <c r="D10">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E10" t="str">
         <f>_xlfn.XLOOKUP(vdW!D10,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ISOPROPANOL</v>
+        <v>2-METHYL-1-PROPANOL</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="str">
         <f>_xlfn.XLOOKUP(vdW!B11,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>2-BUTANOL</v>
+        <v>ISOPROPANOL</v>
       </c>
       <c r="D11">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E11" t="str">
         <f>_xlfn.XLOOKUP(vdW!D11,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>2-BUTANOL</v>
+        <v>ISOPROPANOL</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="str">
         <f>_xlfn.XLOOKUP(vdW!B12,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>2-METHYL-2-PROPANOL</v>
+        <v>2-BUTANOL</v>
       </c>
       <c r="D12">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E12" t="str">
         <f>_xlfn.XLOOKUP(vdW!D12,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>2-METHYL-2-PROPANOL</v>
+        <v>2-BUTANOL</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C13" t="str">
         <f>_xlfn.XLOOKUP(vdW!B13,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>2-METHYL-2-PROPANOL</v>
       </c>
       <c r="D13">
-        <v>503</v>
+        <v>511</v>
       </c>
       <c r="E13" t="str">
         <f>_xlfn.XLOOKUP(vdW!D13,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ETHANOL</v>
-      </c>
-      <c r="G13">
-        <v>25</v>
-      </c>
-      <c r="H13">
-        <v>100.2</v>
-      </c>
-      <c r="I13">
-        <v>17</v>
-      </c>
-      <c r="J13" t="s">
-        <v>160</v>
-      </c>
-      <c r="K13" t="str">
-        <f>_xlfn.XLOOKUP(I13,sources!A$2:A$40,sources!C$2:C$40)</f>
-        <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
+        <v>2-METHYL-2-PROPANOL</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" t="str">
         <f>_xlfn.XLOOKUP(vdW!B14,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>ETHANOL</v>
+        <v>METHANOL</v>
       </c>
       <c r="D14">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="E14" t="str">
         <f>_xlfn.XLOOKUP(vdW!D14,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>ETHANOL</v>
       </c>
       <c r="G14">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="H14">
         <v>100.2</v>
@@ -1774,10 +1814,45 @@
         <v>17</v>
       </c>
       <c r="J14" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="K14" t="str">
         <f>_xlfn.XLOOKUP(I14,sources!A$2:A$40,sources!C$2:C$40)</f>
+        <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="str">
+        <f>_xlfn.XLOOKUP(vdW!B15,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
+        <v>ETHANOL</v>
+      </c>
+      <c r="D15">
+        <v>502</v>
+      </c>
+      <c r="E15" t="str">
+        <f>_xlfn.XLOOKUP(vdW!D15,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
+        <v>METHANOL</v>
+      </c>
+      <c r="G15">
+        <v>35</v>
+      </c>
+      <c r="H15">
+        <v>100.2</v>
+      </c>
+      <c r="I15">
+        <v>17</v>
+      </c>
+      <c r="J15" t="s">
+        <v>154</v>
+      </c>
+      <c r="K15" t="str">
+        <f>_xlfn.XLOOKUP(I15,sources!A$2:A$40,sources!C$2:C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
@@ -1788,286 +1863,270 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2374B1E-7050-450D-B3AF-CF5254FCED57}">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" t="s">
         <v>69</v>
       </c>
-      <c r="D1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>501</v>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>120</v>
+      </c>
+      <c r="M2" t="s">
+        <v>124</v>
+      </c>
+      <c r="N2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="str">
-        <f>_xlfn.XLOOKUP(B3,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>502</v>
-      </c>
-      <c r="E3" t="str">
-        <f>_xlfn.XLOOKUP(D3,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>METHANOL</v>
-      </c>
-      <c r="J3">
-        <v>3.5175999999999999E-2</v>
-      </c>
-      <c r="K3">
-        <v>2899.5</v>
-      </c>
-      <c r="L3">
-        <v>16</v>
-      </c>
-      <c r="N3" t="str">
-        <f>_xlfn.XLOOKUP(L3,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
-        <v>Benchmark1 - distributed with 2.6.5rel</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="str">
         <f>_xlfn.XLOOKUP(B4,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>ETHANOL</v>
+        <v>METHANOL</v>
       </c>
       <c r="D4">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E4" t="str">
         <f>_xlfn.XLOOKUP(D4,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ETHANOL</v>
+        <v>METHANOL</v>
+      </c>
+      <c r="J4">
+        <v>3.5175999999999999E-2</v>
+      </c>
+      <c r="K4">
+        <v>2899.5</v>
+      </c>
+      <c r="L4">
+        <v>16</v>
+      </c>
+      <c r="N4" t="str">
+        <f>_xlfn.XLOOKUP(L4,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
+        <v>Benchmark1 - distributed with 2.6.5rel</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="str">
         <f>_xlfn.XLOOKUP(B5,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1-PROPANOL</v>
+        <v>ETHANOL</v>
       </c>
       <c r="D5">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E5" t="str">
         <f>_xlfn.XLOOKUP(D5,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>1-PROPANOL</v>
+        <v>ETHANOL</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="str">
         <f>_xlfn.XLOOKUP(B6,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1-BUTANOL</v>
+        <v>1-PROPANOL</v>
       </c>
       <c r="D6">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E6" t="str">
         <f>_xlfn.XLOOKUP(D6,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>1-BUTANOL</v>
+        <v>1-PROPANOL</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="str">
         <f>_xlfn.XLOOKUP(B7,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1-PENTANOL</v>
+        <v>1-BUTANOL</v>
       </c>
       <c r="D7">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E7" t="str">
         <f>_xlfn.XLOOKUP(D7,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>1-PENTANOL</v>
+        <v>1-BUTANOL</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.XLOOKUP(B8,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1-HEXANOL</v>
+        <v>1-PENTANOL</v>
       </c>
       <c r="D8">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E8" t="str">
         <f>_xlfn.XLOOKUP(D8,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>1-HEXANOL</v>
+        <v>1-PENTANOL</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="str">
         <f>_xlfn.XLOOKUP(B9,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>2-METHYL-1-PROPANOL</v>
+        <v>1-HEXANOL</v>
       </c>
       <c r="D9">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E9" t="str">
         <f>_xlfn.XLOOKUP(D9,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>2-METHYL-1-PROPANOL</v>
+        <v>1-HEXANOL</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="str">
         <f>_xlfn.XLOOKUP(B10,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>ISOPROPANOL</v>
+        <v>2-METHYL-1-PROPANOL</v>
       </c>
       <c r="D10">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E10" t="str">
         <f>_xlfn.XLOOKUP(D10,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ISOPROPANOL</v>
+        <v>2-METHYL-1-PROPANOL</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="str">
         <f>_xlfn.XLOOKUP(B11,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>2-BUTANOL</v>
+        <v>ISOPROPANOL</v>
       </c>
       <c r="D11">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E11" t="str">
         <f>_xlfn.XLOOKUP(D11,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>2-BUTANOL</v>
+        <v>ISOPROPANOL</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="str">
         <f>_xlfn.XLOOKUP(B12,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>2-METHYL-2-PROPANOL</v>
+        <v>2-BUTANOL</v>
       </c>
       <c r="D12">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E12" t="str">
         <f>_xlfn.XLOOKUP(D12,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>2-METHYL-2-PROPANOL</v>
+        <v>2-BUTANOL</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C13" t="str">
         <f>_xlfn.XLOOKUP(B13,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>2-METHYL-2-PROPANOL</v>
       </c>
       <c r="D13">
-        <v>502</v>
+        <v>511</v>
       </c>
       <c r="E13" t="str">
         <f>_xlfn.XLOOKUP(D13,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>2-METHYL-2-PROPANOL</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" t="str">
         <f>_xlfn.XLOOKUP(B14,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>ETHANOL</v>
+        <v>METHANOL</v>
       </c>
       <c r="D14">
         <v>502</v>
@@ -2079,14 +2138,14 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" t="str">
         <f>_xlfn.XLOOKUP(B15,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>ETHANOL</v>
       </c>
       <c r="D15">
         <v>502</v>
@@ -2095,43 +2154,30 @@
         <f>_xlfn.XLOOKUP(D15,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
         <v>METHANOL</v>
       </c>
-      <c r="J15">
-        <v>3.5180000000000003E-2</v>
-      </c>
-      <c r="K15">
-        <v>2899.5</v>
-      </c>
-      <c r="L15">
-        <v>17</v>
-      </c>
-      <c r="N15" t="str">
-        <f>_xlfn.XLOOKUP(L15,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
-        <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
-      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C16" t="str">
         <f>_xlfn.XLOOKUP(B16,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1,4-DIOXANE</v>
+        <v>METHANOL</v>
       </c>
       <c r="D16">
-        <v>512</v>
+        <v>502</v>
       </c>
       <c r="E16" t="str">
         <f>_xlfn.XLOOKUP(D16,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>CHLOROFORM</v>
+        <v>METHANOL</v>
       </c>
       <c r="J16">
-        <v>0.03</v>
+        <v>3.5180000000000003E-2</v>
       </c>
       <c r="K16">
-        <v>2500</v>
+        <v>2899.5</v>
       </c>
       <c r="L16">
         <v>17</v>
@@ -2143,7 +2189,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <v>12</v>
@@ -2153,17 +2199,17 @@
         <v>1,4-DIOXANE</v>
       </c>
       <c r="D17">
-        <v>502</v>
+        <v>512</v>
       </c>
       <c r="E17" t="str">
         <f>_xlfn.XLOOKUP(D17,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>CHLOROFORM</v>
       </c>
       <c r="J17">
         <v>0.03</v>
       </c>
       <c r="K17">
-        <v>2550</v>
+        <v>2500</v>
       </c>
       <c r="L17">
         <v>17</v>
@@ -2175,7 +2221,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18">
         <v>12</v>
@@ -2185,17 +2231,17 @@
         <v>1,4-DIOXANE</v>
       </c>
       <c r="D18">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="E18" t="str">
         <f>_xlfn.XLOOKUP(D18,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ETHYLENE GLYCOL</v>
+        <v>METHANOL</v>
       </c>
       <c r="J18">
         <v>0.03</v>
       </c>
       <c r="K18">
-        <v>2520</v>
+        <v>2550</v>
       </c>
       <c r="L18">
         <v>17</v>
@@ -2207,7 +2253,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19">
         <v>12</v>
@@ -2217,17 +2263,17 @@
         <v>1,4-DIOXANE</v>
       </c>
       <c r="D19">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E19" t="str">
         <f>_xlfn.XLOOKUP(D19,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>WATER</v>
+        <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="J19">
         <v>0.03</v>
       </c>
       <c r="K19">
-        <v>2300</v>
+        <v>2520</v>
       </c>
       <c r="L19">
         <v>17</v>
@@ -2239,7 +2285,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20">
         <v>12</v>
@@ -2248,18 +2294,18 @@
         <f>_xlfn.XLOOKUP(B20,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
         <v>1,4-DIOXANE</v>
       </c>
-      <c r="F20">
-        <v>1002</v>
-      </c>
-      <c r="G20" t="str">
-        <f>_xlfn.XLOOKUP(F20,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
-        <v>ACETIC ACID</v>
+      <c r="D20">
+        <v>514</v>
+      </c>
+      <c r="E20" t="str">
+        <f>_xlfn.XLOOKUP(D20,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
+        <v>WATER</v>
       </c>
       <c r="J20">
         <v>0.03</v>
       </c>
       <c r="K20">
-        <v>2530</v>
+        <v>2300</v>
       </c>
       <c r="L20">
         <v>17</v>
@@ -2271,27 +2317,27 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C21" t="str">
         <f>_xlfn.XLOOKUP(B21,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>METHANOL</v>
-      </c>
-      <c r="D21">
-        <v>512</v>
-      </c>
-      <c r="E21" t="str">
-        <f>_xlfn.XLOOKUP(D21,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>CHLOROFORM</v>
+        <v>1,4-DIOXANE</v>
+      </c>
+      <c r="F21">
+        <v>1002</v>
+      </c>
+      <c r="G21" t="str">
+        <f>_xlfn.XLOOKUP(F21,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
+        <v>ACETIC ACID</v>
       </c>
       <c r="J21">
         <v>0.03</v>
       </c>
       <c r="K21">
-        <v>2550</v>
+        <v>2530</v>
       </c>
       <c r="L21">
         <v>17</v>
@@ -2303,7 +2349,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -2313,17 +2359,17 @@
         <v>METHANOL</v>
       </c>
       <c r="D22">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E22" t="str">
         <f>_xlfn.XLOOKUP(D22,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ETHYLENE GLYCOL</v>
+        <v>CHLOROFORM</v>
       </c>
       <c r="J22">
         <v>0.03</v>
       </c>
       <c r="K22">
-        <v>2600</v>
+        <v>2550</v>
       </c>
       <c r="L22">
         <v>17</v>
@@ -2335,7 +2381,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2345,17 +2391,17 @@
         <v>METHANOL</v>
       </c>
       <c r="D23">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E23" t="str">
         <f>_xlfn.XLOOKUP(D23,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>WATER</v>
+        <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="J23">
         <v>0.03</v>
       </c>
       <c r="K23">
-        <v>2615</v>
+        <v>2600</v>
       </c>
       <c r="L23">
         <v>17</v>
@@ -2367,7 +2413,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -2376,18 +2422,18 @@
         <f>_xlfn.XLOOKUP(B24,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
         <v>METHANOL</v>
       </c>
-      <c r="F24">
-        <v>1002</v>
-      </c>
-      <c r="G24" t="str">
-        <f>_xlfn.XLOOKUP(F24,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
-        <v>ACETIC ACID</v>
+      <c r="D24">
+        <v>514</v>
+      </c>
+      <c r="E24" t="str">
+        <f>_xlfn.XLOOKUP(D24,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
+        <v>WATER</v>
       </c>
       <c r="J24">
         <v>0.03</v>
       </c>
       <c r="K24">
-        <v>2530</v>
+        <v>2615</v>
       </c>
       <c r="L24">
         <v>17</v>
@@ -2399,27 +2445,27 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C25" t="str">
         <f>_xlfn.XLOOKUP(B25,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>ETHYLENE GLYCOL</v>
-      </c>
-      <c r="D25">
-        <v>512</v>
-      </c>
-      <c r="E25" t="str">
-        <f>_xlfn.XLOOKUP(D25,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>CHLOROFORM</v>
+        <v>METHANOL</v>
+      </c>
+      <c r="F25">
+        <v>1002</v>
+      </c>
+      <c r="G25" t="str">
+        <f>_xlfn.XLOOKUP(F25,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
+        <v>ACETIC ACID</v>
       </c>
       <c r="J25">
         <v>0.03</v>
       </c>
       <c r="K25">
-        <v>2640</v>
+        <v>2530</v>
       </c>
       <c r="L25">
         <v>17</v>
@@ -2431,7 +2477,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26">
         <v>13</v>
@@ -2441,17 +2487,17 @@
         <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="D26">
-        <v>502</v>
+        <v>512</v>
       </c>
       <c r="E26" t="str">
         <f>_xlfn.XLOOKUP(D26,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>CHLOROFORM</v>
       </c>
       <c r="J26">
         <v>0.03</v>
       </c>
       <c r="K26">
-        <v>2540</v>
+        <v>2640</v>
       </c>
       <c r="L26">
         <v>17</v>
@@ -2463,7 +2509,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27">
         <v>13</v>
@@ -2473,17 +2519,17 @@
         <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="D27">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="E27" t="str">
         <f>_xlfn.XLOOKUP(D27,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ETHYLENE GLYCOL</v>
+        <v>METHANOL</v>
       </c>
       <c r="J27">
-        <v>2.4E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K27">
-        <v>2080</v>
+        <v>2540</v>
       </c>
       <c r="L27">
         <v>17</v>
@@ -2495,7 +2541,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28">
         <v>13</v>
@@ -2505,17 +2551,17 @@
         <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="D28">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E28" t="str">
         <f>_xlfn.XLOOKUP(D28,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>WATER</v>
+        <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="J28">
-        <v>0.03</v>
+        <v>2.4E-2</v>
       </c>
       <c r="K28">
-        <v>2650</v>
+        <v>2080</v>
       </c>
       <c r="L28">
         <v>17</v>
@@ -2527,7 +2573,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29">
         <v>13</v>
@@ -2536,18 +2582,18 @@
         <f>_xlfn.XLOOKUP(B29,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
         <v>ETHYLENE GLYCOL</v>
       </c>
-      <c r="F29">
-        <v>1002</v>
-      </c>
-      <c r="G29" t="str">
-        <f>_xlfn.XLOOKUP(F29,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
-        <v>ACETIC ACID</v>
+      <c r="D29">
+        <v>514</v>
+      </c>
+      <c r="E29" t="str">
+        <f>_xlfn.XLOOKUP(D29,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
+        <v>WATER</v>
       </c>
       <c r="J29">
         <v>0.03</v>
       </c>
       <c r="K29">
-        <v>2710</v>
+        <v>2650</v>
       </c>
       <c r="L29">
         <v>17</v>
@@ -2559,27 +2605,27 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30" t="str">
         <f>_xlfn.XLOOKUP(B30,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>WATER</v>
-      </c>
-      <c r="D30">
-        <v>512</v>
-      </c>
-      <c r="E30" t="str">
-        <f>_xlfn.XLOOKUP(D30,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>CHLOROFORM</v>
+        <v>ETHYLENE GLYCOL</v>
+      </c>
+      <c r="F30">
+        <v>1002</v>
+      </c>
+      <c r="G30" t="str">
+        <f>_xlfn.XLOOKUP(F30,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
+        <v>ACETIC ACID</v>
       </c>
       <c r="J30">
         <v>0.03</v>
       </c>
       <c r="K30">
-        <v>2610</v>
+        <v>2710</v>
       </c>
       <c r="L30">
         <v>17</v>
@@ -2591,7 +2637,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31">
         <v>14</v>
@@ -2601,17 +2647,17 @@
         <v>WATER</v>
       </c>
       <c r="D31">
-        <v>502</v>
+        <v>512</v>
       </c>
       <c r="E31" t="str">
         <f>_xlfn.XLOOKUP(D31,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>CHLOROFORM</v>
       </c>
       <c r="J31">
         <v>0.03</v>
       </c>
       <c r="K31">
-        <v>2700</v>
+        <v>2610</v>
       </c>
       <c r="L31">
         <v>17</v>
@@ -2623,7 +2669,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32">
         <v>14</v>
@@ -2633,17 +2679,17 @@
         <v>WATER</v>
       </c>
       <c r="D32">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="E32" t="str">
         <f>_xlfn.XLOOKUP(D32,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ETHYLENE GLYCOL</v>
+        <v>METHANOL</v>
       </c>
       <c r="J32">
         <v>0.03</v>
       </c>
       <c r="K32">
-        <v>2730</v>
+        <v>2700</v>
       </c>
       <c r="L32">
         <v>17</v>
@@ -2655,7 +2701,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33">
         <v>14</v>
@@ -2665,17 +2711,17 @@
         <v>WATER</v>
       </c>
       <c r="D33">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E33" t="str">
         <f>_xlfn.XLOOKUP(D33,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>WATER</v>
+        <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="J33">
-        <v>3.4869999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K33">
-        <v>2500.6999999999998</v>
+        <v>2730</v>
       </c>
       <c r="L33">
         <v>17</v>
@@ -2687,7 +2733,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34">
         <v>14</v>
@@ -2696,18 +2742,18 @@
         <f>_xlfn.XLOOKUP(B34,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
         <v>WATER</v>
       </c>
-      <c r="F34">
-        <v>1002</v>
-      </c>
-      <c r="G34" t="str">
-        <f>_xlfn.XLOOKUP(F34,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
-        <v>ACETIC ACID</v>
+      <c r="D34">
+        <v>514</v>
+      </c>
+      <c r="E34" t="str">
+        <f>_xlfn.XLOOKUP(D34,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
+        <v>WATER</v>
       </c>
       <c r="J34">
-        <v>0.03</v>
+        <v>3.4869999999999998E-2</v>
       </c>
       <c r="K34">
-        <v>2720</v>
+        <v>2500.6999999999998</v>
       </c>
       <c r="L34">
         <v>17</v>
@@ -2719,14 +2765,14 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>32</v>
-      </c>
-      <c r="D35">
-        <v>512</v>
-      </c>
-      <c r="E35" t="str">
-        <f>_xlfn.XLOOKUP(D35,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>CHLOROFORM</v>
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <v>14</v>
+      </c>
+      <c r="C35" t="str">
+        <f>_xlfn.XLOOKUP(B35,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
+        <v>WATER</v>
       </c>
       <c r="F35">
         <v>1002</v>
@@ -2739,7 +2785,7 @@
         <v>0.03</v>
       </c>
       <c r="K35">
-        <v>2560</v>
+        <v>2720</v>
       </c>
       <c r="L35">
         <v>17</v>
@@ -2751,14 +2797,14 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D36">
-        <v>502</v>
+        <v>512</v>
       </c>
       <c r="E36" t="str">
         <f>_xlfn.XLOOKUP(D36,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>CHLOROFORM</v>
       </c>
       <c r="F36">
         <v>1002</v>
@@ -2771,7 +2817,7 @@
         <v>0.03</v>
       </c>
       <c r="K36">
-        <v>2535</v>
+        <v>2560</v>
       </c>
       <c r="L36">
         <v>17</v>
@@ -2783,14 +2829,14 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D37">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="E37" t="str">
         <f>_xlfn.XLOOKUP(D37,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ETHYLENE GLYCOL</v>
+        <v>METHANOL</v>
       </c>
       <c r="F37">
         <v>1002</v>
@@ -2803,7 +2849,7 @@
         <v>0.03</v>
       </c>
       <c r="K37">
-        <v>2800</v>
+        <v>2535</v>
       </c>
       <c r="L37">
         <v>17</v>
@@ -2815,14 +2861,14 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D38">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E38" t="str">
         <f>_xlfn.XLOOKUP(D38,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>WATER</v>
+        <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="F38">
         <v>1002</v>
@@ -2835,7 +2881,7 @@
         <v>0.03</v>
       </c>
       <c r="K38">
-        <v>2730</v>
+        <v>2800</v>
       </c>
       <c r="L38">
         <v>17</v>
@@ -2847,7 +2893,14 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="D39">
+        <v>514</v>
+      </c>
+      <c r="E39" t="str">
+        <f>_xlfn.XLOOKUP(D39,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
+        <v>WATER</v>
       </c>
       <c r="F39">
         <v>1002</v>
@@ -2856,24 +2909,49 @@
         <f>_xlfn.XLOOKUP(F39,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
         <v>ACETIC ACID</v>
       </c>
-      <c r="H39">
-        <v>1002</v>
-      </c>
-      <c r="I39" t="str">
-        <f>_xlfn.XLOOKUP(H39,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
-        <v>ACETIC ACID</v>
-      </c>
       <c r="J39">
-        <v>0.15110000000000001</v>
+        <v>0.03</v>
       </c>
       <c r="K39">
-        <v>3044.4</v>
+        <v>2730</v>
       </c>
       <c r="L39">
         <v>17</v>
       </c>
       <c r="N39" t="str">
         <f>_xlfn.XLOOKUP(L39,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
+        <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>36</v>
+      </c>
+      <c r="F40">
+        <v>1002</v>
+      </c>
+      <c r="G40" t="str">
+        <f>_xlfn.XLOOKUP(F40,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
+        <v>ACETIC ACID</v>
+      </c>
+      <c r="H40">
+        <v>1002</v>
+      </c>
+      <c r="I40" t="str">
+        <f>_xlfn.XLOOKUP(H40,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
+        <v>ACETIC ACID</v>
+      </c>
+      <c r="J40">
+        <v>0.15110000000000001</v>
+      </c>
+      <c r="K40">
+        <v>3044.4</v>
+      </c>
+      <c r="L40">
+        <v>17</v>
+      </c>
+      <c r="N40" t="str">
+        <f>_xlfn.XLOOKUP(L40,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>
@@ -2894,42 +2972,42 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
       <c r="K2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -2966,7 +3044,7 @@
         <v>0.47</v>
       </c>
       <c r="K3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L3">
         <v>16</v>
@@ -3010,7 +3088,7 @@
         <v>0.3</v>
       </c>
       <c r="K4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L4">
         <v>16</v>
@@ -3054,7 +3132,7 @@
         <v>0.3</v>
       </c>
       <c r="K5" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="L5">
         <v>17</v>
@@ -3098,7 +3176,7 @@
         <v>0.3</v>
       </c>
       <c r="K6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L6">
         <v>17</v>
@@ -3142,7 +3220,7 @@
         <v>0.3</v>
       </c>
       <c r="K7" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L7">
         <v>17</v>
@@ -3170,13 +3248,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" t="s">
         <v>89</v>
-      </c>
-      <c r="B1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -3184,10 +3262,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -3195,10 +3273,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -3206,10 +3284,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -3217,7 +3295,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -3225,10 +3303,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -3236,10 +3314,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -3247,10 +3325,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -3258,10 +3336,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -3269,10 +3347,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -3280,10 +3358,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -3291,10 +3369,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -3302,7 +3380,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -3310,10 +3388,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -3321,10 +3399,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -3332,10 +3410,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -3343,7 +3421,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -3351,7 +3429,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -3359,10 +3437,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -3386,57 +3464,57 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="H1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>137</v>
-      </c>
-      <c r="H2" t="s">
-        <v>138</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
       <c r="L2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="N2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -4194,34 +4272,34 @@
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" t="s">
         <v>143</v>
-      </c>
-      <c r="E2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G2" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2" t="s">
-        <v>147</v>
-      </c>
-      <c r="I2" t="s">
-        <v>148</v>
-      </c>
-      <c r="J2" t="s">
-        <v>149</v>
       </c>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
@@ -4543,7 +4621,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:E16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4559,7 +4637,7 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -4570,16 +4648,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" t="s">
         <v>130</v>
-      </c>
-      <c r="E2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -4587,10 +4665,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>180</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -4601,7 +4679,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>168</v>
       </c>
       <c r="C4">
         <v>5350</v>
@@ -4619,7 +4697,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>169</v>
       </c>
       <c r="C5">
         <v>5245</v>
@@ -4637,7 +4715,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>170</v>
       </c>
       <c r="C6">
         <v>5514</v>
@@ -4655,7 +4733,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>171</v>
       </c>
       <c r="C7">
         <v>5520</v>
@@ -4673,7 +4751,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>172</v>
       </c>
       <c r="C8">
         <v>5521</v>
@@ -4691,7 +4769,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>173</v>
       </c>
       <c r="C9">
         <v>742</v>
@@ -4709,7 +4787,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>174</v>
       </c>
       <c r="C10">
         <v>5892</v>
@@ -4727,7 +4805,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>175</v>
       </c>
       <c r="C11">
         <v>5352</v>
@@ -4745,7 +4823,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>181</v>
       </c>
       <c r="C12">
         <v>5898</v>
@@ -4763,7 +4841,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>176</v>
       </c>
       <c r="C13">
         <v>5673</v>
@@ -4781,7 +4859,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>131</v>
+        <v>178</v>
       </c>
       <c r="C14">
         <v>1122</v>
@@ -4799,7 +4877,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>177</v>
       </c>
       <c r="C15">
         <v>7609</v>
@@ -4817,7 +4895,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="C16">
         <v>5822</v>
@@ -4840,7 +4918,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:E16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4856,7 +4934,7 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -4867,16 +4945,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -4884,10 +4962,10 @@
         <v>501</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>156</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -4898,7 +4976,7 @@
         <v>502</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>155</v>
       </c>
       <c r="C4">
         <v>5350</v>
@@ -4916,7 +4994,7 @@
         <v>503</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>157</v>
       </c>
       <c r="C5">
         <v>5245</v>
@@ -4934,7 +5012,7 @@
         <v>504</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>158</v>
       </c>
       <c r="C6">
         <v>5514</v>
@@ -4952,7 +5030,7 @@
         <v>505</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>159</v>
       </c>
       <c r="C7">
         <v>5520</v>
@@ -4970,7 +5048,7 @@
         <v>506</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>160</v>
       </c>
       <c r="C8">
         <v>5521</v>
@@ -4988,7 +5066,7 @@
         <v>507</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>161</v>
       </c>
       <c r="C9">
         <v>742</v>
@@ -5006,7 +5084,7 @@
         <v>508</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>162</v>
       </c>
       <c r="C10">
         <v>5892</v>
@@ -5024,7 +5102,7 @@
         <v>509</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>163</v>
       </c>
       <c r="C11">
         <v>5352</v>
@@ -5042,7 +5120,7 @@
         <v>510</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C12">
         <v>5898</v>
@@ -5060,7 +5138,7 @@
         <v>511</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>164</v>
       </c>
       <c r="C13">
         <v>5673</v>
@@ -5078,7 +5156,7 @@
         <v>512</v>
       </c>
       <c r="B14" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="C14">
         <v>5355</v>
@@ -5096,7 +5174,7 @@
         <v>513</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>166</v>
       </c>
       <c r="C15">
         <v>7609</v>
@@ -5114,7 +5192,7 @@
         <v>514</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>167</v>
       </c>
       <c r="C16">
         <v>5822</v>
@@ -5137,7 +5215,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5153,7 +5231,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -5164,16 +5242,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -5181,10 +5259,10 @@
         <v>1001</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -5192,7 +5270,7 @@
         <v>1002</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>182</v>
       </c>
       <c r="C4">
         <v>5247</v>
@@ -5212,11 +5290,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601862DE-66FD-4FF3-953E-01550CFBC136}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -5226,96 +5302,69 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" t="s">
         <v>69</v>
       </c>
-      <c r="D1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>123</v>
-      </c>
-      <c r="K1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>501</v>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="str">
-        <f>_xlfn.XLOOKUP(gconst!B3,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>502</v>
-      </c>
-      <c r="E3" t="str">
-        <f>_xlfn.XLOOKUP(gconst!D3,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>METHANOL</v>
-      </c>
-      <c r="H3">
-        <v>1.7609999999999999</v>
-      </c>
-      <c r="I3">
-        <v>2590.9</v>
-      </c>
-      <c r="J3">
-        <v>18</v>
-      </c>
-      <c r="K3" t="str">
-        <f>_xlfn.XLOOKUP(J3,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
-        <v>W.G. Killian, A.T. Norfleet, L. Peereboom, C.T. Lira, Fourier Transform Infrared Spectroscopy Applied to Association Modeling of Binary Alcohol + Cyclohexane Mixtures, Ind. Eng. Chem. Res. 62 (2023) 14620–14637. https://doi.org/10.1021/acs.iecr.3c00968.</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="str">
         <f>_xlfn.XLOOKUP(gconst!B4,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>ETHANOL</v>
+        <v>METHANOL</v>
       </c>
       <c r="D4">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E4" t="str">
         <f>_xlfn.XLOOKUP(gconst!D4,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ETHANOL</v>
+        <v>METHANOL</v>
       </c>
       <c r="H4">
-        <v>0.86487000000000003</v>
+        <v>1.7609999999999999</v>
       </c>
       <c r="I4">
-        <v>2685.2</v>
+        <v>2590.9</v>
       </c>
       <c r="J4">
         <v>18</v>
@@ -5327,27 +5376,27 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="str">
         <f>_xlfn.XLOOKUP(gconst!B5,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1-PROPANOL</v>
+        <v>ETHANOL</v>
       </c>
       <c r="D5">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E5" t="str">
         <f>_xlfn.XLOOKUP(gconst!D5,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>1-PROPANOL</v>
+        <v>ETHANOL</v>
       </c>
       <c r="H5">
-        <v>0.91622999999999999</v>
+        <v>0.86487000000000003</v>
       </c>
       <c r="I5">
-        <v>2704.1</v>
+        <v>2685.2</v>
       </c>
       <c r="J5">
         <v>18</v>
@@ -5359,27 +5408,27 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="str">
         <f>_xlfn.XLOOKUP(gconst!B6,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1-BUTANOL</v>
+        <v>1-PROPANOL</v>
       </c>
       <c r="D6">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E6" t="str">
         <f>_xlfn.XLOOKUP(gconst!D6,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>1-BUTANOL</v>
+        <v>1-PROPANOL</v>
       </c>
       <c r="H6">
-        <v>0.84923000000000004</v>
+        <v>0.91622999999999999</v>
       </c>
       <c r="I6">
-        <v>2723.9</v>
+        <v>2704.1</v>
       </c>
       <c r="J6">
         <v>18</v>
@@ -5391,27 +5440,27 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="str">
         <f>_xlfn.XLOOKUP(gconst!B7,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1-PENTANOL</v>
+        <v>1-BUTANOL</v>
       </c>
       <c r="D7">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E7" t="str">
         <f>_xlfn.XLOOKUP(gconst!D7,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>1-PENTANOL</v>
+        <v>1-BUTANOL</v>
       </c>
       <c r="H7">
-        <v>0.67127000000000003</v>
+        <v>0.84923000000000004</v>
       </c>
       <c r="I7">
-        <v>2816.1</v>
+        <v>2723.9</v>
       </c>
       <c r="J7">
         <v>18</v>
@@ -5423,27 +5472,27 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.XLOOKUP(gconst!B8,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1-HEXANOL</v>
+        <v>1-PENTANOL</v>
       </c>
       <c r="D8">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E8" t="str">
         <f>_xlfn.XLOOKUP(gconst!D8,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>1-HEXANOL</v>
+        <v>1-PENTANOL</v>
       </c>
       <c r="H8">
-        <v>0.80767</v>
+        <v>0.67127000000000003</v>
       </c>
       <c r="I8">
-        <v>2763.2</v>
+        <v>2816.1</v>
       </c>
       <c r="J8">
         <v>18</v>
@@ -5455,27 +5504,27 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="str">
         <f>_xlfn.XLOOKUP(gconst!B9,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>2-METHYL-1-PROPANOL</v>
+        <v>1-HEXANOL</v>
       </c>
       <c r="D9">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E9" t="str">
         <f>_xlfn.XLOOKUP(gconst!D9,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>2-METHYL-1-PROPANOL</v>
+        <v>1-HEXANOL</v>
       </c>
       <c r="H9">
-        <v>0.83050999999999997</v>
+        <v>0.80767</v>
       </c>
       <c r="I9">
-        <v>2717</v>
+        <v>2763.2</v>
       </c>
       <c r="J9">
         <v>18</v>
@@ -5487,27 +5536,27 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="str">
         <f>_xlfn.XLOOKUP(gconst!B10,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>ISOPROPANOL</v>
+        <v>2-METHYL-1-PROPANOL</v>
       </c>
       <c r="D10">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E10" t="str">
         <f>_xlfn.XLOOKUP(gconst!D10,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ISOPROPANOL</v>
+        <v>2-METHYL-1-PROPANOL</v>
       </c>
       <c r="H10">
-        <v>0.94781000000000004</v>
+        <v>0.83050999999999997</v>
       </c>
       <c r="I10">
-        <v>2724.5</v>
+        <v>2717</v>
       </c>
       <c r="J10">
         <v>18</v>
@@ -5519,27 +5568,27 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="str">
         <f>_xlfn.XLOOKUP(gconst!B11,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>2-BUTANOL</v>
+        <v>ISOPROPANOL</v>
       </c>
       <c r="D11">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E11" t="str">
         <f>_xlfn.XLOOKUP(gconst!D11,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>2-BUTANOL</v>
+        <v>ISOPROPANOL</v>
       </c>
       <c r="H11">
-        <v>0.59067999999999998</v>
+        <v>0.94781000000000004</v>
       </c>
       <c r="I11">
-        <v>2762.1</v>
+        <v>2724.5</v>
       </c>
       <c r="J11">
         <v>18</v>
@@ -5551,33 +5600,65 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="str">
         <f>_xlfn.XLOOKUP(gconst!B12,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>2-METHYL-2-PROPANOL</v>
+        <v>2-BUTANOL</v>
       </c>
       <c r="D12">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E12" t="str">
         <f>_xlfn.XLOOKUP(gconst!D12,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>2-METHYL-2-PROPANOL</v>
+        <v>2-BUTANOL</v>
       </c>
       <c r="H12">
-        <v>0.54157999999999995</v>
+        <v>0.59067999999999998</v>
       </c>
       <c r="I12">
-        <v>2725.8</v>
+        <v>2762.1</v>
       </c>
       <c r="J12">
         <v>18</v>
       </c>
       <c r="K12" t="str">
         <f>_xlfn.XLOOKUP(J12,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
+        <v>W.G. Killian, A.T. Norfleet, L. Peereboom, C.T. Lira, Fourier Transform Infrared Spectroscopy Applied to Association Modeling of Binary Alcohol + Cyclohexane Mixtures, Ind. Eng. Chem. Res. 62 (2023) 14620–14637. https://doi.org/10.1021/acs.iecr.3c00968.</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" t="str">
+        <f>_xlfn.XLOOKUP(gconst!B13,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
+        <v>2-METHYL-2-PROPANOL</v>
+      </c>
+      <c r="D13">
+        <v>511</v>
+      </c>
+      <c r="E13" t="str">
+        <f>_xlfn.XLOOKUP(gconst!D13,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
+        <v>2-METHYL-2-PROPANOL</v>
+      </c>
+      <c r="H13">
+        <v>0.54157999999999995</v>
+      </c>
+      <c r="I13">
+        <v>2725.8</v>
+      </c>
+      <c r="J13">
+        <v>18</v>
+      </c>
+      <c r="K13" t="str">
+        <f>_xlfn.XLOOKUP(J13,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>W.G. Killian, A.T. Norfleet, L. Peereboom, C.T. Lira, Fourier Transform Infrared Spectroscopy Applied to Association Modeling of Binary Alcohol + Cyclohexane Mixtures, Ind. Eng. Chem. Res. 62 (2023) 14620–14637. https://doi.org/10.1021/acs.iecr.3c00968.</v>
       </c>
     </row>
@@ -5589,312 +5670,283 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CBBE5A-E8DE-4E54-B78F-49BA95C635AD}">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:L37"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" t="s">
         <v>69</v>
       </c>
-      <c r="D1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>501</v>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>121</v>
+      </c>
+      <c r="M2" t="s">
+        <v>124</v>
+      </c>
+      <c r="N2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="str">
-        <f>_xlfn.XLOOKUP(B3,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>502</v>
-      </c>
-      <c r="E3" t="str">
-        <f>_xlfn.XLOOKUP(D3,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>METHANOL</v>
-      </c>
-      <c r="J3">
-        <v>0.49748999999999999</v>
-      </c>
-      <c r="K3">
-        <v>2957.6</v>
-      </c>
-      <c r="L3">
-        <v>16</v>
-      </c>
-      <c r="N3" t="str">
-        <f>_xlfn.XLOOKUP(L3,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
-        <v>Benchmark1 - distributed with 2.6.5rel</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="str">
         <f>_xlfn.XLOOKUP(B4,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>ETHANOL</v>
+        <v>METHANOL</v>
       </c>
       <c r="D4">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E4" t="str">
         <f>_xlfn.XLOOKUP(D4,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ETHANOL</v>
+        <v>METHANOL</v>
+      </c>
+      <c r="J4">
+        <v>0.49748999999999999</v>
+      </c>
+      <c r="K4">
+        <v>2957.6</v>
+      </c>
+      <c r="L4">
+        <v>16</v>
+      </c>
+      <c r="N4" t="str">
+        <f>_xlfn.XLOOKUP(L4,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
+        <v>Benchmark1 - distributed with 2.6.5rel</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="str">
         <f>_xlfn.XLOOKUP(B5,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1-PROPANOL</v>
+        <v>ETHANOL</v>
       </c>
       <c r="D5">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E5" t="str">
         <f>_xlfn.XLOOKUP(D5,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>1-PROPANOL</v>
+        <v>ETHANOL</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="str">
         <f>_xlfn.XLOOKUP(B6,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1-BUTANOL</v>
+        <v>1-PROPANOL</v>
       </c>
       <c r="D6">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E6" t="str">
         <f>_xlfn.XLOOKUP(D6,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>1-BUTANOL</v>
+        <v>1-PROPANOL</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="str">
         <f>_xlfn.XLOOKUP(B7,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1-PENTANOL</v>
+        <v>1-BUTANOL</v>
       </c>
       <c r="D7">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E7" t="str">
         <f>_xlfn.XLOOKUP(D7,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>1-PENTANOL</v>
+        <v>1-BUTANOL</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.XLOOKUP(B8,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1-HEXANOL</v>
+        <v>1-PENTANOL</v>
       </c>
       <c r="D8">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E8" t="str">
         <f>_xlfn.XLOOKUP(D8,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>1-HEXANOL</v>
+        <v>1-PENTANOL</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="str">
         <f>_xlfn.XLOOKUP(B9,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>2-METHYL-1-PROPANOL</v>
+        <v>1-HEXANOL</v>
       </c>
       <c r="D9">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E9" t="str">
         <f>_xlfn.XLOOKUP(D9,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>2-METHYL-1-PROPANOL</v>
+        <v>1-HEXANOL</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="str">
         <f>_xlfn.XLOOKUP(B10,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>ISOPROPANOL</v>
+        <v>2-METHYL-1-PROPANOL</v>
       </c>
       <c r="D10">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E10" t="str">
         <f>_xlfn.XLOOKUP(D10,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ISOPROPANOL</v>
+        <v>2-METHYL-1-PROPANOL</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="str">
         <f>_xlfn.XLOOKUP(B11,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>2-BUTANOL</v>
+        <v>ISOPROPANOL</v>
       </c>
       <c r="D11">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E11" t="str">
         <f>_xlfn.XLOOKUP(D11,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>2-BUTANOL</v>
+        <v>ISOPROPANOL</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="str">
         <f>_xlfn.XLOOKUP(B12,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>2-METHYL-2-PROPANOL</v>
+        <v>2-BUTANOL</v>
       </c>
       <c r="D12">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E12" t="str">
         <f>_xlfn.XLOOKUP(D12,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>2-METHYL-2-PROPANOL</v>
+        <v>2-BUTANOL</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C13" t="str">
         <f>_xlfn.XLOOKUP(B13,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>2-METHYL-2-PROPANOL</v>
       </c>
       <c r="D13">
-        <v>502</v>
+        <v>511</v>
       </c>
       <c r="E13" t="str">
         <f>_xlfn.XLOOKUP(D13,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>METHANOL</v>
-      </c>
-      <c r="J13">
-        <v>0.49748999999999999</v>
-      </c>
-      <c r="K13">
-        <v>2957.6</v>
-      </c>
-      <c r="L13">
-        <v>17</v>
-      </c>
-      <c r="N13" t="str">
-        <f>_xlfn.XLOOKUP(L13,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
-        <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
+        <v>2-METHYL-2-PROPANOL</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C14" t="str">
         <f>_xlfn.XLOOKUP(B14,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>1,4-DIOXANE</v>
+        <v>METHANOL</v>
       </c>
       <c r="D14">
-        <v>512</v>
+        <v>502</v>
       </c>
       <c r="E14" t="str">
         <f>_xlfn.XLOOKUP(D14,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>CHLOROFORM</v>
+        <v>METHANOL</v>
       </c>
       <c r="J14">
-        <v>1.0995600000000001</v>
+        <v>0.49748999999999999</v>
       </c>
       <c r="K14">
         <v>2957.6</v>
@@ -5909,7 +5961,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>12</v>
@@ -5919,14 +5971,14 @@
         <v>1,4-DIOXANE</v>
       </c>
       <c r="D15">
-        <v>502</v>
+        <v>512</v>
       </c>
       <c r="E15" t="str">
         <f>_xlfn.XLOOKUP(D15,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>CHLOROFORM</v>
       </c>
       <c r="J15">
-        <v>0.74952700000000005</v>
+        <v>1.0995600000000001</v>
       </c>
       <c r="K15">
         <v>2957.6</v>
@@ -5941,7 +5993,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>12</v>
@@ -5951,17 +6003,17 @@
         <v>1,4-DIOXANE</v>
       </c>
       <c r="D16">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="E16" t="str">
         <f>_xlfn.XLOOKUP(D16,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ETHYLENE GLYCOL</v>
+        <v>METHANOL</v>
       </c>
       <c r="J16">
-        <v>0.90466199999999997</v>
+        <v>0.74952700000000005</v>
       </c>
       <c r="K16">
-        <v>2666.61</v>
+        <v>2957.6</v>
       </c>
       <c r="L16">
         <v>17</v>
@@ -5973,7 +6025,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>12</v>
@@ -5983,17 +6035,17 @@
         <v>1,4-DIOXANE</v>
       </c>
       <c r="D17">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E17" t="str">
         <f>_xlfn.XLOOKUP(D17,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>WATER</v>
+        <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="J17">
-        <v>1.06447</v>
+        <v>0.90466199999999997</v>
       </c>
       <c r="K17">
-        <v>2480.37</v>
+        <v>2666.61</v>
       </c>
       <c r="L17">
         <v>17</v>
@@ -6005,7 +6057,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>12</v>
@@ -6014,18 +6066,18 @@
         <f>_xlfn.XLOOKUP(B18,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
         <v>1,4-DIOXANE</v>
       </c>
-      <c r="F18">
-        <v>1002</v>
-      </c>
-      <c r="G18" t="str">
-        <f>_xlfn.XLOOKUP(F18,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
-        <v>ACETIC ACID</v>
+      <c r="D18">
+        <v>514</v>
+      </c>
+      <c r="E18" t="str">
+        <f>_xlfn.XLOOKUP(D18,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
+        <v>WATER</v>
       </c>
       <c r="J18">
-        <v>0.48766799999999999</v>
+        <v>1.06447</v>
       </c>
       <c r="K18">
-        <v>3903.66</v>
+        <v>2480.37</v>
       </c>
       <c r="L18">
         <v>17</v>
@@ -6037,27 +6089,27 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C19" t="str">
         <f>_xlfn.XLOOKUP(B19,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>METHANOL</v>
-      </c>
-      <c r="D19">
-        <v>512</v>
-      </c>
-      <c r="E19" t="str">
-        <f>_xlfn.XLOOKUP(D19,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>CHLOROFORM</v>
+        <v>1,4-DIOXANE</v>
+      </c>
+      <c r="F19">
+        <v>1002</v>
+      </c>
+      <c r="G19" t="str">
+        <f>_xlfn.XLOOKUP(F19,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
+        <v>ACETIC ACID</v>
       </c>
       <c r="J19">
-        <v>0.72982000000000002</v>
+        <v>0.48766799999999999</v>
       </c>
       <c r="K19">
-        <v>2957.6</v>
+        <v>3903.66</v>
       </c>
       <c r="L19">
         <v>17</v>
@@ -6069,7 +6121,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -6079,17 +6131,17 @@
         <v>METHANOL</v>
       </c>
       <c r="D20">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E20" t="str">
         <f>_xlfn.XLOOKUP(D20,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ETHYLENE GLYCOL</v>
+        <v>CHLOROFORM</v>
       </c>
       <c r="J20">
-        <v>0.60045899999999996</v>
+        <v>0.72982000000000002</v>
       </c>
       <c r="K20">
-        <v>2666.61</v>
+        <v>2957.6</v>
       </c>
       <c r="L20">
         <v>17</v>
@@ -6101,7 +6153,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -6111,17 +6163,17 @@
         <v>METHANOL</v>
       </c>
       <c r="D21">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E21" t="str">
         <f>_xlfn.XLOOKUP(D21,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>WATER</v>
+        <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="J21">
-        <v>0.70652800000000004</v>
+        <v>0.60045899999999996</v>
       </c>
       <c r="K21">
-        <v>2480.37</v>
+        <v>2666.61</v>
       </c>
       <c r="L21">
         <v>17</v>
@@ -6133,7 +6185,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -6142,18 +6194,18 @@
         <f>_xlfn.XLOOKUP(B22,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
         <v>METHANOL</v>
       </c>
-      <c r="F22">
-        <v>1002</v>
-      </c>
-      <c r="G22" t="str">
-        <f>_xlfn.XLOOKUP(F22,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
-        <v>ACETIC ACID</v>
+      <c r="D22">
+        <v>514</v>
+      </c>
+      <c r="E22" t="str">
+        <f>_xlfn.XLOOKUP(D22,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
+        <v>WATER</v>
       </c>
       <c r="J22">
-        <v>0.32368400000000003</v>
+        <v>0.70652800000000004</v>
       </c>
       <c r="K22">
-        <v>3903.66</v>
+        <v>2480.37</v>
       </c>
       <c r="L22">
         <v>17</v>
@@ -6165,27 +6217,27 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C23" t="str">
         <f>_xlfn.XLOOKUP(B23,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>ETHYLENE GLYCOL</v>
-      </c>
-      <c r="D23">
-        <v>512</v>
-      </c>
-      <c r="E23" t="str">
-        <f>_xlfn.XLOOKUP(D23,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>CHLOROFORM</v>
+        <v>METHANOL</v>
+      </c>
+      <c r="F23">
+        <v>1002</v>
+      </c>
+      <c r="G23" t="str">
+        <f>_xlfn.XLOOKUP(F23,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
+        <v>ACETIC ACID</v>
       </c>
       <c r="J23">
-        <v>0.88087599999999999</v>
+        <v>0.32368400000000003</v>
       </c>
       <c r="K23">
-        <v>2666.61</v>
+        <v>3903.66</v>
       </c>
       <c r="L23">
         <v>17</v>
@@ -6197,7 +6249,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>13</v>
@@ -6207,14 +6259,14 @@
         <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="D24">
-        <v>502</v>
+        <v>512</v>
       </c>
       <c r="E24" t="str">
         <f>_xlfn.XLOOKUP(D24,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>CHLOROFORM</v>
       </c>
       <c r="J24">
-        <v>0.60045899999999996</v>
+        <v>0.88087599999999999</v>
       </c>
       <c r="K24">
         <v>2666.61</v>
@@ -6229,7 +6281,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>13</v>
@@ -6239,17 +6291,17 @@
         <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="D25">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="E25" t="str">
         <f>_xlfn.XLOOKUP(D25,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ETHYLENE GLYCOL</v>
+        <v>METHANOL</v>
       </c>
       <c r="J25">
-        <v>0.72474000000000005</v>
+        <v>0.60045899999999996</v>
       </c>
       <c r="K25">
-        <v>2375.61</v>
+        <v>2666.61</v>
       </c>
       <c r="L25">
         <v>17</v>
@@ -6261,7 +6313,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>13</v>
@@ -6271,17 +6323,17 @@
         <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="D26">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E26" t="str">
         <f>_xlfn.XLOOKUP(D26,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>WATER</v>
+        <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="J26">
-        <v>0.85276300000000005</v>
+        <v>0.72474000000000005</v>
       </c>
       <c r="K26">
-        <v>2189.37</v>
+        <v>2375.61</v>
       </c>
       <c r="L26">
         <v>17</v>
@@ -6293,7 +6345,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>13</v>
@@ -6302,18 +6354,18 @@
         <f>_xlfn.XLOOKUP(B27,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
         <v>ETHYLENE GLYCOL</v>
       </c>
-      <c r="F27">
-        <v>1002</v>
-      </c>
-      <c r="G27" t="str">
-        <f>_xlfn.XLOOKUP(F27,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
-        <v>ACETIC ACID</v>
+      <c r="D27">
+        <v>514</v>
+      </c>
+      <c r="E27" t="str">
+        <f>_xlfn.XLOOKUP(D27,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
+        <v>WATER</v>
       </c>
       <c r="J27">
-        <v>0.390679</v>
+        <v>0.85276300000000005</v>
       </c>
       <c r="K27">
-        <v>3612.66</v>
+        <v>2189.37</v>
       </c>
       <c r="L27">
         <v>17</v>
@@ -6325,27 +6377,27 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" t="str">
         <f>_xlfn.XLOOKUP(B28,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
-        <v>WATER</v>
-      </c>
-      <c r="D28">
-        <v>512</v>
-      </c>
-      <c r="E28" t="str">
-        <f>_xlfn.XLOOKUP(D28,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>CHLOROFORM</v>
+        <v>ETHYLENE GLYCOL</v>
+      </c>
+      <c r="F28">
+        <v>1002</v>
+      </c>
+      <c r="G28" t="str">
+        <f>_xlfn.XLOOKUP(F28,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
+        <v>ACETIC ACID</v>
       </c>
       <c r="J28">
-        <v>1.0364800000000001</v>
+        <v>0.390679</v>
       </c>
       <c r="K28">
-        <v>2480.37</v>
+        <v>3612.66</v>
       </c>
       <c r="L28">
         <v>17</v>
@@ -6357,7 +6409,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>14</v>
@@ -6367,14 +6419,14 @@
         <v>WATER</v>
       </c>
       <c r="D29">
-        <v>502</v>
+        <v>512</v>
       </c>
       <c r="E29" t="str">
         <f>_xlfn.XLOOKUP(D29,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>CHLOROFORM</v>
       </c>
       <c r="J29">
-        <v>0.70652800000000004</v>
+        <v>1.0364800000000001</v>
       </c>
       <c r="K29">
         <v>2480.37</v>
@@ -6389,7 +6441,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>14</v>
@@ -6399,17 +6451,17 @@
         <v>WATER</v>
       </c>
       <c r="D30">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="E30" t="str">
         <f>_xlfn.XLOOKUP(D30,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ETHYLENE GLYCOL</v>
+        <v>METHANOL</v>
       </c>
       <c r="J30">
-        <v>0.85276300000000005</v>
+        <v>0.70652800000000004</v>
       </c>
       <c r="K30">
-        <v>2189.37</v>
+        <v>2480.37</v>
       </c>
       <c r="L30">
         <v>17</v>
@@ -6421,7 +6473,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>14</v>
@@ -6431,17 +6483,17 @@
         <v>WATER</v>
       </c>
       <c r="D31">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E31" t="str">
         <f>_xlfn.XLOOKUP(D31,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>WATER</v>
+        <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="J31">
-        <v>1.0034000000000001</v>
+        <v>0.85276300000000005</v>
       </c>
       <c r="K31">
-        <v>2003.13</v>
+        <v>2189.37</v>
       </c>
       <c r="L31">
         <v>17</v>
@@ -6453,7 +6505,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>14</v>
@@ -6462,18 +6514,18 @@
         <f>_xlfn.XLOOKUP(B32,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
         <v>WATER</v>
       </c>
-      <c r="F32">
-        <v>1002</v>
-      </c>
-      <c r="G32" t="str">
-        <f>_xlfn.XLOOKUP(F32,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
-        <v>ACETIC ACID</v>
+      <c r="D32">
+        <v>514</v>
+      </c>
+      <c r="E32" t="str">
+        <f>_xlfn.XLOOKUP(D32,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
+        <v>WATER</v>
       </c>
       <c r="J32">
-        <v>0.45969100000000002</v>
+        <v>1.0034000000000001</v>
       </c>
       <c r="K32">
-        <v>3426.42</v>
+        <v>2003.13</v>
       </c>
       <c r="L32">
         <v>17</v>
@@ -6485,14 +6537,14 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="D33">
-        <v>512</v>
-      </c>
-      <c r="E33" t="str">
-        <f>_xlfn.XLOOKUP(D33,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>CHLOROFORM</v>
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>14</v>
+      </c>
+      <c r="C33" t="str">
+        <f>_xlfn.XLOOKUP(B33,ed!$A$2:$A$500,ed!$D$2:$D$500)</f>
+        <v>WATER</v>
       </c>
       <c r="F33">
         <v>1002</v>
@@ -6502,10 +6554,10 @@
         <v>ACETIC ACID</v>
       </c>
       <c r="J33">
-        <v>0.47484599999999999</v>
+        <v>0.45969100000000002</v>
       </c>
       <c r="K33">
-        <v>3903.66</v>
+        <v>3426.42</v>
       </c>
       <c r="L33">
         <v>17</v>
@@ -6517,14 +6569,14 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D34">
-        <v>502</v>
+        <v>512</v>
       </c>
       <c r="E34" t="str">
         <f>_xlfn.XLOOKUP(D34,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>METHANOL</v>
+        <v>CHLOROFORM</v>
       </c>
       <c r="F34">
         <v>1002</v>
@@ -6534,7 +6586,7 @@
         <v>ACETIC ACID</v>
       </c>
       <c r="J34">
-        <v>0.32368400000000003</v>
+        <v>0.47484599999999999</v>
       </c>
       <c r="K34">
         <v>3903.66</v>
@@ -6549,14 +6601,14 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="E35" t="str">
         <f>_xlfn.XLOOKUP(D35,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>ETHYLENE GLYCOL</v>
+        <v>METHANOL</v>
       </c>
       <c r="F35">
         <v>1002</v>
@@ -6566,10 +6618,10 @@
         <v>ACETIC ACID</v>
       </c>
       <c r="J35">
-        <v>0.390679</v>
+        <v>0.32368400000000003</v>
       </c>
       <c r="K35">
-        <v>3612.66</v>
+        <v>3903.66</v>
       </c>
       <c r="L35">
         <v>17</v>
@@ -6581,14 +6633,14 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E36" t="str">
         <f>_xlfn.XLOOKUP(D36,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
-        <v>WATER</v>
+        <v>ETHYLENE GLYCOL</v>
       </c>
       <c r="F36">
         <v>1002</v>
@@ -6598,10 +6650,10 @@
         <v>ACETIC ACID</v>
       </c>
       <c r="J36">
-        <v>0.45969100000000002</v>
+        <v>0.390679</v>
       </c>
       <c r="K36">
-        <v>3426.42</v>
+        <v>3612.66</v>
       </c>
       <c r="L36">
         <v>17</v>
@@ -6613,7 +6665,14 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="D37">
+        <v>514</v>
+      </c>
+      <c r="E37" t="str">
+        <f>_xlfn.XLOOKUP(D37,ea!$A$2:$A$500,ea!$D$2:$D$500)</f>
+        <v>WATER</v>
       </c>
       <c r="F37">
         <v>1002</v>
@@ -6622,24 +6681,49 @@
         <f>_xlfn.XLOOKUP(F37,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
         <v>ACETIC ACID</v>
       </c>
-      <c r="H37">
-        <v>1002</v>
-      </c>
-      <c r="I37" t="str">
-        <f>_xlfn.XLOOKUP(H37,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
-        <v>ACETIC ACID</v>
-      </c>
       <c r="J37">
-        <v>0.21060000000000001</v>
+        <v>0.45969100000000002</v>
       </c>
       <c r="K37">
-        <v>4849.72</v>
+        <v>3426.42</v>
       </c>
       <c r="L37">
         <v>17</v>
       </c>
       <c r="N37" t="str">
         <f>_xlfn.XLOOKUP(L37,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
+        <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="F38">
+        <v>1002</v>
+      </c>
+      <c r="G38" t="str">
+        <f>_xlfn.XLOOKUP(F38,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
+        <v>ACETIC ACID</v>
+      </c>
+      <c r="H38">
+        <v>1002</v>
+      </c>
+      <c r="I38" t="str">
+        <f>_xlfn.XLOOKUP(H38,eda!$A$2:$A$500,eda!$D$2:$D$500)</f>
+        <v>ACETIC ACID</v>
+      </c>
+      <c r="J38">
+        <v>0.21060000000000001</v>
+      </c>
+      <c r="K38">
+        <v>4849.72</v>
+      </c>
+      <c r="L38">
+        <v>17</v>
+      </c>
+      <c r="N38" t="str">
+        <f>_xlfn.XLOOKUP(L38,sources!$A$2:$A$40,sources!$C$2:$C$40)</f>
         <v>Benchmark2 - internal test document, random (unrealistic) parameter values to test code</v>
       </c>
     </row>

</xml_diff>